<commit_message>
Them ham xep theo alpha, chinh tong alpha = 12
</commit_message>
<xml_diff>
--- a/alpha.xlsx
+++ b/alpha.xlsx
@@ -416,10 +416,13 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I23"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="52" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -474,7 +477,11 @@
           <t>C# Winform</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -482,40 +489,54 @@
           <t>Công nghệ Java</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Công nghệ thiết kế Web</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
+          <t>Công nghệ thiết kế WEB</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Công nghệ thiết kế Web nâng cao</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5</v>
+          <t>Công nghệ thiết kế WEB nâng cao</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -524,8 +545,15 @@
           <t>Đồ án Công nghệ thiết kế Web nâng cao</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>5</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="F6" t="n">
         <v>5</v>
@@ -537,8 +565,10 @@
           <t>Đồ án Phát triển cho ứng dụng di động</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E7" t="n">
         <v>5</v>
@@ -550,8 +580,10 @@
           <t>Phát triển cho ứng dụng di động</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>5</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E8" t="n">
         <v>5</v>
@@ -563,8 +595,10 @@
           <t>Đồ án công nghệ phần mềm</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>10</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -573,11 +607,15 @@
           <t>Cấu trúc dữ liệu và thuật toán</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" t="n">
-        <v>5</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -586,11 +624,15 @@
           <t>Cấu trúc dữ liệu và thuật toán 1</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -599,8 +641,10 @@
           <t>Công nghệ phần mềm</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>10</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -609,8 +653,10 @@
           <t>Công nghệ Web</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>10</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -619,8 +665,10 @@
           <t>Cơ sở dữ liệu nâng cao</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>10</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -629,8 +677,10 @@
           <t>Phần mềm nguồn mở</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>10</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -639,11 +689,20 @@
           <t>Đồ án hệ cơ sở dữ liệu</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>5</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -652,11 +711,15 @@
           <t>Đồ án phân tích và thiết kế hệ thống thông tin</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="I17" t="n">
         <v>4</v>
@@ -668,11 +731,15 @@
           <t>Hệ cơ sở dữ liệu</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>5</v>
-      </c>
-      <c r="H18" t="n">
-        <v>5</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -681,11 +748,15 @@
           <t>Phân tích và thiết kế hệ thống thông tin</t>
         </is>
       </c>
-      <c r="G19" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" t="n">
-        <v>3</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="I19" t="n">
         <v>4</v>
@@ -697,8 +768,10 @@
           <t>Lập trình LINUX</t>
         </is>
       </c>
-      <c r="H20" t="n">
-        <v>10</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -707,8 +780,10 @@
           <t>Quản lý dự án công nghệ thông tin</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>10</v>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -717,8 +792,10 @@
           <t>Thiết kế giao diện và tương tác người máy</t>
         </is>
       </c>
-      <c r="I22" t="n">
-        <v>10</v>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -727,8 +804,10 @@
           <t>Lập trình Web</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>10</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>